<commit_message>
transfer from gitlab to github
</commit_message>
<xml_diff>
--- a/forecast_data.xlsx
+++ b/forecast_data.xlsx
@@ -466,20 +466,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-05-04T16:00+00:00</t>
+          <t>2024-10-09T12:00+00:00</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16736851.2</v>
+        <v>3811062</v>
       </c>
       <c r="D2" t="n">
-        <v>15.7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F2" t="n">
-        <v>1.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -488,20 +488,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-05-04T17:00+00:00</t>
+          <t>2024-10-09T13:00+00:00</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>16874672</v>
+        <v>4694910</v>
       </c>
       <c r="D3" t="n">
-        <v>14.5</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.3</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="4">
@@ -510,20 +510,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-05-04T18:00+00:00</t>
+          <t>2024-10-09T14:00+00:00</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>17096265.6</v>
+        <v>5489148</v>
       </c>
       <c r="D4" t="n">
-        <v>13.2</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.2</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="5">
@@ -532,20 +532,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-05-04T19:00+00:00</t>
+          <t>2024-10-09T15:00+00:00</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17100320</v>
+        <v>6156986</v>
       </c>
       <c r="D5" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.3</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="6">
@@ -554,20 +554,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-05-04T20:00+00:00</t>
+          <t>2024-10-09T16:00+00:00</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>17100320</v>
+        <v>6441854</v>
       </c>
       <c r="D6" t="n">
-        <v>12.5</v>
+        <v>8.4</v>
       </c>
       <c r="E6" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.6</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="7">
@@ -576,20 +576,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-05-04T21:00+00:00</t>
+          <t>2024-10-09T17:00+00:00</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17100320</v>
+        <v>6456946</v>
       </c>
       <c r="D7" t="n">
-        <v>9.6</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="8">
@@ -598,20 +598,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-05-04T22:00+00:00</t>
+          <t>2024-10-09T18:00+00:00</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17100320</v>
+        <v>6456946</v>
       </c>
       <c r="D8" t="n">
-        <v>9.6</v>
+        <v>8.1</v>
       </c>
       <c r="E8" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.5</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="9">
@@ -620,20 +620,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-05-04T23:00+00:00</t>
+          <t>2024-10-09T19:00+00:00</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17100320</v>
+        <v>6456946</v>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>8.6</v>
       </c>
       <c r="E9" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.5</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="10">
@@ -642,20 +642,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-05-05T00:00+00:00</t>
+          <t>2024-10-09T20:00+00:00</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17100320</v>
+        <v>6456946</v>
       </c>
       <c r="D10" t="n">
-        <v>6.7</v>
+        <v>8.9</v>
       </c>
       <c r="E10" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.9</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="11">
@@ -664,20 +664,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-05-05T01:00+00:00</t>
+          <t>2024-10-09T21:00+00:00</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>17100320</v>
+        <v>6456946</v>
       </c>
       <c r="D11" t="n">
-        <v>5.7</v>
+        <v>9.1</v>
       </c>
       <c r="E11" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -686,20 +686,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-05-05T02:00+00:00</t>
+          <t>2024-10-09T22:00+00:00</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17100320</v>
+        <v>6456946</v>
       </c>
       <c r="D12" t="n">
-        <v>5.1</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E12" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.6</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="13">
@@ -708,20 +708,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-05-05T03:00+00:00</t>
+          <t>2024-10-09T23:00+00:00</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>17100320</v>
+        <v>6456946</v>
       </c>
       <c r="D13" t="n">
-        <v>4.5</v>
+        <v>9.5</v>
       </c>
       <c r="E13" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.6</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="14">
@@ -730,20 +730,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-05-05T04:00+00:00</t>
+          <t>2024-10-10T00:00+00:00</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>17112480</v>
+        <v>6456946</v>
       </c>
       <c r="D14" t="n">
-        <v>4.3</v>
+        <v>9.1</v>
       </c>
       <c r="E14" t="n">
-        <v>12640.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.5</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="15">
@@ -752,20 +752,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-05-05T05:00+00:00</t>
+          <t>2024-10-10T01:00+00:00</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17486755.2</v>
+        <v>6456946</v>
       </c>
       <c r="D15" t="n">
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
       <c r="E15" t="n">
-        <v>16000.3</v>
+        <v>2352.8</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.4</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="16">
@@ -774,20 +774,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-05-05T06:00+00:00</t>
+          <t>2024-10-10T02:00+00:00</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>18512302.4</v>
+        <v>6456946</v>
       </c>
       <c r="D16" t="n">
-        <v>10.9</v>
+        <v>9</v>
       </c>
       <c r="E16" t="n">
-        <v>19240.9</v>
+        <v>2352.8</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="17">
@@ -796,20 +796,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-05-05T07:00+00:00</t>
+          <t>2024-10-10T03:00+00:00</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>20193168</v>
+        <v>6456946</v>
       </c>
       <c r="D17" t="n">
-        <v>13</v>
+        <v>8.6</v>
       </c>
       <c r="E17" t="n">
-        <v>22495.2</v>
+        <v>2352.8</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.2</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="18">
@@ -818,20 +818,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-05-05T08:00+00:00</t>
+          <t>2024-10-10T04:00+00:00</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>22488822.4</v>
+        <v>6456946</v>
       </c>
       <c r="D18" t="n">
-        <v>14.9</v>
+        <v>8.5</v>
       </c>
       <c r="E18" t="n">
-        <v>25827.6</v>
+        <v>2352.8</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="19">
@@ -840,20 +840,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-05-05T09:00+00:00</t>
+          <t>2024-10-10T05:00+00:00</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>25319544</v>
+        <v>6456946</v>
       </c>
       <c r="D19" t="n">
-        <v>17.5</v>
+        <v>8.4</v>
       </c>
       <c r="E19" t="n">
-        <v>29169.7</v>
+        <v>2352.8</v>
       </c>
       <c r="F19" t="n">
-        <v>0.3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="20">
@@ -862,20 +862,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-05-05T10:00+00:00</t>
+          <t>2024-10-10T06:00+00:00</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>28432659.2</v>
+        <v>6480528</v>
       </c>
       <c r="D20" t="n">
-        <v>19.8</v>
+        <v>8.4</v>
       </c>
       <c r="E20" t="n">
-        <v>32174.2</v>
+        <v>2352.8</v>
       </c>
       <c r="F20" t="n">
-        <v>1.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -884,20 +884,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-05-05T11:00+00:00</t>
+          <t>2024-10-10T07:00+00:00</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>31620092.8</v>
+        <v>6608814</v>
       </c>
       <c r="D21" t="n">
-        <v>20.9</v>
+        <v>8.9</v>
       </c>
       <c r="E21" t="n">
-        <v>34661.8</v>
+        <v>2352.8</v>
       </c>
       <c r="F21" t="n">
-        <v>1.6</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="22">
@@ -906,20 +906,20 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-05-05T12:00+00:00</t>
+          <t>2024-10-10T08:00+00:00</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>34758880</v>
+        <v>7062528</v>
       </c>
       <c r="D22" t="n">
-        <v>21.3</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E22" t="n">
-        <v>36093.8</v>
+        <v>2352.8</v>
       </c>
       <c r="F22" t="n">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="23">
@@ -928,20 +928,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-05-05T13:00+00:00</t>
+          <t>2024-10-10T09:00+00:00</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>37612572.8</v>
+        <v>7765268</v>
       </c>
       <c r="D23" t="n">
-        <v>21.4</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="E23" t="n">
-        <v>37648.8</v>
+        <v>2352.8</v>
       </c>
       <c r="F23" t="n">
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="24">
@@ -950,20 +950,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-05-05T14:00+00:00</t>
+          <t>2024-10-10T10:00+00:00</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>39740678.4</v>
+        <v>8748160</v>
       </c>
       <c r="D24" t="n">
-        <v>21.1</v>
+        <v>9.6</v>
       </c>
       <c r="E24" t="n">
-        <v>37648.8</v>
+        <v>2352.8</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -972,20 +972,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-05-05T15:00+00:00</t>
+          <t>2024-10-10T11:00+00:00</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>41067539.2</v>
+        <v>9038689.6</v>
       </c>
       <c r="D25" t="n">
-        <v>19.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E25" t="n">
-        <v>37648.8</v>
+        <v>2352.8</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.7</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="26">
@@ -994,20 +994,20 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-05-05T16:00+00:00</t>
+          <t>2024-10-10T12:00+00:00</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>41759344</v>
+        <v>9345253.6</v>
       </c>
       <c r="D26" t="n">
-        <v>16.6</v>
+        <v>10.8</v>
       </c>
       <c r="E26" t="n">
-        <v>38109.2</v>
+        <v>2352.8</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>